<commit_message>
更新依賴，充實 README.md Update the dependencies, enrich README.md.
</commit_message>
<xml_diff>
--- a/install/src/languages.xlsx
+++ b/install/src/languages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Python\VoiceInput\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BE8B91-3A30-4C92-A9D9-185642038254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F035E527-1C9C-4579-8B13-3405D476FAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3043" yWindow="0" windowWidth="17158" windowHeight="14672" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3002" yWindow="0" windowWidth="14971" windowHeight="13952" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
   <si>
     <t>key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -350,6 +350,18 @@
   </si>
   <si>
     <t>zh-TW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>toggle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Toggle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>切換</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -759,13 +771,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
@@ -1103,6 +1115,17 @@
       </c>
       <c r="C30" s="1" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>